<commit_message>
ver6.7 update index.html and script.js
</commit_message>
<xml_diff>
--- a/screenings.xlsx
+++ b/screenings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F209FD0-1944-4FB1-BB6F-B5E8CF3F1EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DB5A38-A420-4C5E-A79F-7B33243048AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{010CC3F0-DFCB-4839-9665-95B8E91DA0C2}"/>
   </bookViews>
@@ -660,9 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DE6ECF-7C70-4084-966B-7420C68F1251}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -706,69 +704,69 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
+        <v>80</v>
+      </c>
+      <c r="E3" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
-        <v>100</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D4" s="3">
+        <v>100</v>
+      </c>
+      <c r="E4" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>80</v>
-      </c>
-      <c r="E4" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E5" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E6" s="3">
         <v>25</v>
@@ -776,16 +774,16 @@
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="3">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E7" s="3">
         <v>25</v>
@@ -793,30 +791,30 @@
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E8" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3">
         <v>150</v>
@@ -825,18 +823,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E10" s="3">
         <v>25</v>
@@ -844,27 +842,27 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
         <v>150</v>
       </c>
       <c r="E11" s="3">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -873,55 +871,55 @@
         <v>150</v>
       </c>
       <c r="E12" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E13" s="3">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="D14" s="3">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E14" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E15" s="3">
         <v>25</v>
@@ -929,101 +927,101 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3">
+        <v>150</v>
+      </c>
+      <c r="E16" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3">
+        <v>100</v>
+      </c>
+      <c r="E18" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3">
+        <v>100</v>
+      </c>
+      <c r="E19" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3">
-        <v>100</v>
-      </c>
-      <c r="E16" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3">
+        <v>100</v>
+      </c>
+      <c r="E20" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="3">
-        <v>100</v>
-      </c>
-      <c r="E17" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3">
-        <v>120</v>
-      </c>
-      <c r="E18" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3">
-        <v>150</v>
-      </c>
-      <c r="E19" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3">
-        <v>100</v>
-      </c>
-      <c r="E20" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D21" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E21" s="3">
         <v>25</v>
@@ -1031,33 +1029,33 @@
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="3">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E22" s="3">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E23" s="3">
         <v>25</v>
@@ -1065,10 +1063,10 @@
     </row>
     <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>10</v>
@@ -1082,13 +1080,13 @@
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="D25" s="3">
         <v>150</v>
@@ -1099,10 +1097,10 @@
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
@@ -1114,12 +1112,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>10</v>
@@ -1133,10 +1131,10 @@
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
@@ -1150,13 +1148,13 @@
     </row>
     <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3">
         <v>150</v>
@@ -1167,10 +1165,10 @@
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>10</v>
@@ -1184,13 +1182,13 @@
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D31" s="3">
         <v>100</v>
@@ -1201,13 +1199,13 @@
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D32" s="3">
         <v>100</v>
@@ -1218,10 +1216,10 @@
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>10</v>
@@ -1230,89 +1228,89 @@
         <v>150</v>
       </c>
       <c r="E33" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E34" s="3">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="D35" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E35" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E36" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E37" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="C38" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="3">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E38" s="3">
         <v>35</v>
@@ -1320,19 +1318,19 @@
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D39" s="3">
         <v>150</v>
       </c>
       <c r="E39" s="3">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1353,6 +1351,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
+    <sortCondition ref="A1:A40"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ver6.7.1 update screening excel
</commit_message>
<xml_diff>
--- a/screenings.xlsx
+++ b/screenings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DB5A38-A420-4C5E-A79F-7B33243048AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6704BA-773C-4C68-AA2F-18A1314EE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{010CC3F0-DFCB-4839-9665-95B8E91DA0C2}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>East</t>
   </si>
   <si>
-    <t>Location Name</t>
-  </si>
-  <si>
     <t>Price (SGD)</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>Cafe Football (East Coast Park)</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -684,18 +684,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3">
         <v>150</v>
@@ -706,13 +706,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3">
         <v>80</v>
@@ -723,13 +723,13 @@
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="3">
         <v>100</v>
@@ -740,10 +740,10 @@
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -757,13 +757,13 @@
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3">
         <v>150</v>
@@ -774,13 +774,13 @@
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="3">
         <v>150</v>
@@ -791,13 +791,13 @@
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -808,13 +808,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3">
         <v>150</v>
@@ -825,13 +825,13 @@
     </row>
     <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="3">
         <v>150</v>
@@ -842,10 +842,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -859,13 +859,13 @@
     </row>
     <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3">
         <v>150</v>
@@ -876,13 +876,13 @@
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="3">
         <v>150</v>
@@ -893,13 +893,13 @@
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3">
         <v>150</v>
@@ -910,10 +910,10 @@
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -927,13 +927,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="3">
         <v>150</v>
@@ -944,13 +944,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" s="3">
         <v>100</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D18" s="3">
         <v>100</v>
@@ -978,13 +978,13 @@
     </row>
     <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="3">
         <v>100</v>
@@ -995,13 +995,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="3">
         <v>100</v>
@@ -1012,10 +1012,10 @@
     </row>
     <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -1029,13 +1029,13 @@
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3">
         <v>120</v>
@@ -1046,13 +1046,13 @@
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D23" s="3">
         <v>150</v>
@@ -1063,13 +1063,13 @@
     </row>
     <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" s="3">
         <v>100</v>
@@ -1080,13 +1080,13 @@
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25" s="3">
         <v>150</v>
@@ -1097,13 +1097,13 @@
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D26" s="3">
         <v>100</v>
@@ -1114,13 +1114,13 @@
     </row>
     <row r="27" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D27" s="3">
         <v>100</v>
@@ -1131,13 +1131,13 @@
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" s="3">
         <v>100</v>
@@ -1148,13 +1148,13 @@
     </row>
     <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D29" s="3">
         <v>150</v>
@@ -1165,13 +1165,13 @@
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30" s="3">
         <v>100</v>
@@ -1182,13 +1182,13 @@
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31" s="3">
         <v>100</v>
@@ -1199,13 +1199,13 @@
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="3">
         <v>100</v>
@@ -1216,13 +1216,13 @@
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" s="3">
         <v>150</v>
@@ -1233,13 +1233,13 @@
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="C34" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D34" s="3">
         <v>100</v>
@@ -1250,10 +1250,10 @@
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -1284,13 +1284,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C37" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D37" s="3">
         <v>100</v>
@@ -1301,13 +1301,13 @@
     </row>
     <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C38" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38" s="3">
         <v>200</v>
@@ -1318,13 +1318,13 @@
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="C39" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D39" s="3">
         <v>150</v>

</xml_diff>

<commit_message>
ver6.9 update screening excel price and about html
</commit_message>
<xml_diff>
--- a/screenings.xlsx
+++ b/screenings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6704BA-773C-4C68-AA2F-18A1314EE22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE314682-CFAD-4227-AC15-BB0025E5DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{010CC3F0-DFCB-4839-9665-95B8E91DA0C2}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>East</t>
   </si>
   <si>
-    <t>Price (SGD)</t>
-  </si>
-  <si>
     <t>Al Capone's Sports Bar &amp; Dining</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Est. Price Per Pax (SGD)</t>
   </si>
 </sst>
 </file>
@@ -660,19 +660,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DE6ECF-7C70-4084-966B-7420C68F1251}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="34.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="15.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -684,18 +686,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3">
         <v>150</v>
@@ -706,13 +708,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3">
         <v>80</v>
@@ -723,13 +725,13 @@
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="3">
         <v>100</v>
@@ -740,10 +742,10 @@
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -757,13 +759,13 @@
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="3">
         <v>150</v>
@@ -774,13 +776,13 @@
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3">
         <v>150</v>
@@ -791,13 +793,13 @@
     </row>
     <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -808,13 +810,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3">
         <v>150</v>
@@ -825,13 +827,13 @@
     </row>
     <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3">
         <v>150</v>
@@ -842,10 +844,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -859,13 +861,13 @@
     </row>
     <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="3">
         <v>150</v>
@@ -876,13 +878,13 @@
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
         <v>150</v>
@@ -893,13 +895,13 @@
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3">
         <v>150</v>
@@ -910,10 +912,10 @@
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -927,13 +929,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3">
         <v>150</v>
@@ -944,13 +946,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3">
         <v>100</v>
@@ -961,13 +963,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3">
         <v>100</v>
@@ -978,13 +980,13 @@
     </row>
     <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="3">
         <v>100</v>
@@ -995,13 +997,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20" s="3">
         <v>100</v>
@@ -1012,10 +1014,10 @@
     </row>
     <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -1029,13 +1031,13 @@
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="3">
         <v>120</v>
@@ -1046,13 +1048,13 @@
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D23" s="3">
         <v>150</v>
@@ -1063,13 +1065,13 @@
     </row>
     <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24" s="3">
         <v>100</v>
@@ -1080,13 +1082,13 @@
     </row>
     <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" s="3">
         <v>150</v>
@@ -1097,13 +1099,13 @@
     </row>
     <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="C26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26" s="3">
         <v>100</v>
@@ -1114,13 +1116,13 @@
     </row>
     <row r="27" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C27" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27" s="3">
         <v>100</v>
@@ -1131,13 +1133,13 @@
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="C28" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="3">
         <v>100</v>
@@ -1148,13 +1150,13 @@
     </row>
     <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="D29" s="3">
         <v>150</v>
@@ -1165,13 +1167,13 @@
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3">
         <v>100</v>
@@ -1182,13 +1184,13 @@
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="C31" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="3">
         <v>100</v>
@@ -1199,13 +1201,13 @@
     </row>
     <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C32" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="3">
         <v>100</v>
@@ -1216,13 +1218,13 @@
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="C33" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33" s="3">
         <v>150</v>
@@ -1233,13 +1235,13 @@
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="C34" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="3">
         <v>100</v>
@@ -1250,10 +1252,10 @@
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -1267,10 +1269,10 @@
     </row>
     <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -1284,13 +1286,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C37" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37" s="3">
         <v>100</v>
@@ -1301,13 +1303,13 @@
     </row>
     <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="C38" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D38" s="3">
         <v>200</v>
@@ -1318,13 +1320,13 @@
     </row>
     <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="C39" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D39" s="3">
         <v>150</v>

</xml_diff>

<commit_message>
ver7.2 update screening excel
</commit_message>
<xml_diff>
--- a/screenings.xlsx
+++ b/screenings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE314682-CFAD-4227-AC15-BB0025E5DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368BD719-D23A-4B41-BBE5-8AE2FCB2F40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{010CC3F0-DFCB-4839-9665-95B8E91DA0C2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t>Address</t>
   </si>
@@ -205,18 +205,6 @@
   </si>
   <si>
     <t>238 Thomson Road, #01-59/60, Novena Square, Singapore 307683</t>
-  </si>
-  <si>
-    <t>Harry's Plaza Singapura</t>
-  </si>
-  <si>
-    <t>68 Orchard Road, #01-50, Plaza Singapura, Singapore 238839</t>
-  </si>
-  <si>
-    <t>Harry's Riverside Point</t>
-  </si>
-  <si>
-    <t>30 Merchant Road, #01-04, Singapore 058282</t>
   </si>
   <si>
     <t>Harry's South Beach Avenue</t>
@@ -658,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DE6ECF-7C70-4084-966B-7420C68F1251}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A32" sqref="A32:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,7 +662,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -686,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -844,10 +832,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -861,10 +849,10 @@
     </row>
     <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -878,10 +866,10 @@
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
@@ -895,10 +883,10 @@
     </row>
     <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>55</v>
@@ -912,10 +900,10 @@
     </row>
     <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -929,10 +917,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -1017,7 +1005,7 @@
         <v>38</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -1218,16 +1206,16 @@
     </row>
     <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D33" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E33" s="3">
         <v>25</v>
@@ -1235,13 +1223,13 @@
     </row>
     <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D34" s="3">
         <v>100</v>
@@ -1250,111 +1238,77 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D35" s="3">
         <v>100</v>
       </c>
       <c r="E35" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="3">
+        <v>200</v>
+      </c>
+      <c r="E36" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3">
+        <v>150</v>
+      </c>
+      <c r="E37" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="3">
-        <v>100</v>
-      </c>
-      <c r="E36" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="3">
-        <v>100</v>
-      </c>
-      <c r="E37" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="3">
+      <c r="D38" s="5">
         <v>200</v>
       </c>
-      <c r="E38" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="3">
-        <v>150</v>
-      </c>
-      <c r="E39" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3</v>
-      </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="5">
-        <v>200</v>
-      </c>
-      <c r="E40" s="5">
+      <c r="E38" s="5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
-    <sortCondition ref="A1:A40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
+    <sortCondition ref="A1:A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>